<commit_message>
fixing yr1957 nangler data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb117/raw/Table22.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb117/raw/Table22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb117/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83918BBE-A53E-4347-BF88-4C0BD0DC156E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C793D8E-D11F-914E-92C8-AE6FF9A652CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Linccod</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total number of fish </t>
-  </si>
-  <si>
-    <t>662069,</t>
   </si>
   <si>
     <t>Barracuda, California</t>
@@ -89,7 +86,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -146,32 +143,32 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -491,7 +488,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,7 +502,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3">
         <v>1951</v>
@@ -575,7 +572,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="6">
         <v>269545</v>
@@ -610,7 +607,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>14475</v>
@@ -645,7 +642,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>59295</v>
@@ -680,7 +677,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5">
         <v>781609</v>
@@ -750,7 +747,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>721808</v>
@@ -785,7 +782,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="6">
         <v>71970</v>
@@ -820,7 +817,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="6">
         <v>44367</v>
@@ -855,7 +852,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6">
         <v>35721</v>
@@ -890,7 +887,7 @@
     </row>
     <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>23721</v>
@@ -925,7 +922,7 @@
     </row>
     <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6">
         <v>228157</v>
@@ -995,7 +992,7 @@
     </row>
     <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6">
         <v>687721</v>
@@ -1015,8 +1012,8 @@
       <c r="G15" s="6">
         <v>645878</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>3</v>
+      <c r="H15" s="6">
+        <v>662069</v>
       </c>
       <c r="I15" s="7">
         <v>636110</v>
@@ -1030,7 +1027,7 @@
     </row>
     <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="11">
         <f>SUM(B2:B13)-B14</f>

</xml_diff>